<commit_message>
Add entries to challenges map
</commit_message>
<xml_diff>
--- a/src/resources/templates/excel/challenges_map.xlsx
+++ b/src/resources/templates/excel/challenges_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249550FC-CB53-427C-B8D9-C24E03553F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079216B1-0FB3-486A-A7E6-2905BADD2330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Challenge Name</t>
   </si>
@@ -36,14 +36,44 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>URL to Learn More</t>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Hiring technical staff</t>
+  </si>
+  <si>
+    <t>SME-QA</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>https://www.usds.gov/projects/smeqa</t>
+  </si>
+  <si>
+    <t>https://www.opm.gov/policy-data-oversight/hiring-information/intergovernment-personnel-act/</t>
+  </si>
+  <si>
+    <t>18F</t>
+  </si>
+  <si>
+    <t>TMF</t>
+  </si>
+  <si>
+    <t>https://tmf.cio.gov/</t>
+  </si>
+  <si>
+    <t>https://18f.gsa.gov/</t>
+  </si>
+  <si>
+    <t>Inadequate technical solutions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +85,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,19 +136,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -124,6 +170,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,15 +439,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +474,58 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
+    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F9F4FD07-3953-45E1-BEF5-8D16586ADC7C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{659B25B2-B605-42AE-9B47-14A9C84D0604}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{59C94EEE-EC7D-4F22-A882-EBFD19CCAF43}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{F8C3D682-340B-4B05-BB8B-F13596E19516}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>